<commit_message>
Till 1000 rows script results
</commit_message>
<xml_diff>
--- a/Addresses.xlsx
+++ b/Addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pycharm Projects\Upwork\Employee_Assign_Addresses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBAB75B-1E2D-4873-BE85-9C475FC054C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F6467A-DF99-4E39-A6F9-2AFE275D1AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="832">
   <si>
     <t>Address</t>
   </si>
@@ -1590,6 +1590,933 @@
   </si>
   <si>
     <t>61107-5754</t>
+  </si>
+  <si>
+    <t>100 N Cross Pointe Blvd</t>
+  </si>
+  <si>
+    <t>Evansville</t>
+  </si>
+  <si>
+    <t>47715-2797</t>
+  </si>
+  <si>
+    <t>3645 River Crossing Pkwy</t>
+  </si>
+  <si>
+    <t>Indianapolis</t>
+  </si>
+  <si>
+    <t>46240-2192</t>
+  </si>
+  <si>
+    <t>455 Commerce Rd</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>47374-2646</t>
+  </si>
+  <si>
+    <t>110 Huntington Ave</t>
+  </si>
+  <si>
+    <t>02116-5706</t>
+  </si>
+  <si>
+    <t>47 Huntington Ave</t>
+  </si>
+  <si>
+    <t>02116-5728</t>
+  </si>
+  <si>
+    <t>1694 Falmouth Rd</t>
+  </si>
+  <si>
+    <t>Centerville</t>
+  </si>
+  <si>
+    <t>02632-2933</t>
+  </si>
+  <si>
+    <t>124 Womack Dr</t>
+  </si>
+  <si>
+    <t>21401-7399</t>
+  </si>
+  <si>
+    <t>201 Wye Woods Dr</t>
+  </si>
+  <si>
+    <t>Queenstown</t>
+  </si>
+  <si>
+    <t>21658-1564</t>
+  </si>
+  <si>
+    <t>1 Choice Hotels Cir Ste 400</t>
+  </si>
+  <si>
+    <t>Rockville</t>
+  </si>
+  <si>
+    <t>20850-5172</t>
+  </si>
+  <si>
+    <t>9421 Largo Dr W</t>
+  </si>
+  <si>
+    <t>Upper Marlboro</t>
+  </si>
+  <si>
+    <t>20774-4759</t>
+  </si>
+  <si>
+    <t>Po Box 457</t>
+  </si>
+  <si>
+    <t>Jackman</t>
+  </si>
+  <si>
+    <t>04945-0457</t>
+  </si>
+  <si>
+    <t>6444 Telegraph Rd</t>
+  </si>
+  <si>
+    <t>Erie</t>
+  </si>
+  <si>
+    <t>48133-9432</t>
+  </si>
+  <si>
+    <t>3704 Vanrick Dr</t>
+  </si>
+  <si>
+    <t>49001-0807</t>
+  </si>
+  <si>
+    <t>601 N Huron Ave</t>
+  </si>
+  <si>
+    <t>Mackinaw City</t>
+  </si>
+  <si>
+    <t>49701-9693</t>
+  </si>
+  <si>
+    <t>1019 Paul Bunyan Dr S</t>
+  </si>
+  <si>
+    <t>Bemidji</t>
+  </si>
+  <si>
+    <t>56601-3223</t>
+  </si>
+  <si>
+    <t>701 Carlson Pkwy</t>
+  </si>
+  <si>
+    <t>Hopkins</t>
+  </si>
+  <si>
+    <t>55305-5237</t>
+  </si>
+  <si>
+    <t>701 Carlson Pkwy Ste 600</t>
+  </si>
+  <si>
+    <t>55305-5244</t>
+  </si>
+  <si>
+    <t>1802 Gamel Cemetery Rd</t>
+  </si>
+  <si>
+    <t>Festus</t>
+  </si>
+  <si>
+    <t>63028-2303</t>
+  </si>
+  <si>
+    <t>5404 Osage Beach Pkwy</t>
+  </si>
+  <si>
+    <t>Osage Beach</t>
+  </si>
+  <si>
+    <t>65065-3045</t>
+  </si>
+  <si>
+    <t>6390 Us Highway 93 S</t>
+  </si>
+  <si>
+    <t>Whitefish</t>
+  </si>
+  <si>
+    <t>59937-8235</t>
+  </si>
+  <si>
+    <t>901 Albemarle Rd</t>
+  </si>
+  <si>
+    <t>Asheboro</t>
+  </si>
+  <si>
+    <t>27203-6147</t>
+  </si>
+  <si>
+    <t>85 Pinecrest Ln</t>
+  </si>
+  <si>
+    <t>Tryon</t>
+  </si>
+  <si>
+    <t>28782-3486</t>
+  </si>
+  <si>
+    <t>33 Dow Ave</t>
+  </si>
+  <si>
+    <t>Franconia</t>
+  </si>
+  <si>
+    <t>03580-4915</t>
+  </si>
+  <si>
+    <t>703 River Rd</t>
+  </si>
+  <si>
+    <t>Plainfield</t>
+  </si>
+  <si>
+    <t>03781-5044</t>
+  </si>
+  <si>
+    <t>805 Stockton Ave</t>
+  </si>
+  <si>
+    <t>Cape May</t>
+  </si>
+  <si>
+    <t>08204-2446</t>
+  </si>
+  <si>
+    <t>900 Delsea Dr N</t>
+  </si>
+  <si>
+    <t>Glassboro</t>
+  </si>
+  <si>
+    <t>08028-1440</t>
+  </si>
+  <si>
+    <t>1409 Black Horse Pike</t>
+  </si>
+  <si>
+    <t>Hammonton</t>
+  </si>
+  <si>
+    <t>08037-2831</t>
+  </si>
+  <si>
+    <t>224 Middle Rd Ste 3</t>
+  </si>
+  <si>
+    <t>Hazlet</t>
+  </si>
+  <si>
+    <t>07730-1900</t>
+  </si>
+  <si>
+    <t>1 Hilton Ct</t>
+  </si>
+  <si>
+    <t>Parsippany</t>
+  </si>
+  <si>
+    <t>07054-4403</t>
+  </si>
+  <si>
+    <t>299 Smith Rd</t>
+  </si>
+  <si>
+    <t>07054-2803</t>
+  </si>
+  <si>
+    <t>3 Gatehall Dr</t>
+  </si>
+  <si>
+    <t>07054-4513</t>
+  </si>
+  <si>
+    <t>200 Fred Wehran Dr</t>
+  </si>
+  <si>
+    <t>Teterboro</t>
+  </si>
+  <si>
+    <t>07608-1132</t>
+  </si>
+  <si>
+    <t>401 E 21st Ave</t>
+  </si>
+  <si>
+    <t>Wildwood</t>
+  </si>
+  <si>
+    <t>08260-5323</t>
+  </si>
+  <si>
+    <t>604 Agua Fria St</t>
+  </si>
+  <si>
+    <t>Santa Fe</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>87501-2577</t>
+  </si>
+  <si>
+    <t>Highway 50 &amp; Highway 6</t>
+  </si>
+  <si>
+    <t>Baker</t>
+  </si>
+  <si>
+    <t>200 Oak St</t>
+  </si>
+  <si>
+    <t>Batavia</t>
+  </si>
+  <si>
+    <t>14020-1032</t>
+  </si>
+  <si>
+    <t>129 County Highway 110</t>
+  </si>
+  <si>
+    <t>Broadalbin</t>
+  </si>
+  <si>
+    <t>12025-3201</t>
+  </si>
+  <si>
+    <t>348 Sunside Rd</t>
+  </si>
+  <si>
+    <t>East Durham</t>
+  </si>
+  <si>
+    <t>12423-1636</t>
+  </si>
+  <si>
+    <t>222 S Cayuga St</t>
+  </si>
+  <si>
+    <t>14850-5510</t>
+  </si>
+  <si>
+    <t>32 Star Island Rd</t>
+  </si>
+  <si>
+    <t>Montauk</t>
+  </si>
+  <si>
+    <t>11954-5271</t>
+  </si>
+  <si>
+    <t>6 York St</t>
+  </si>
+  <si>
+    <t>7 Times Sq</t>
+  </si>
+  <si>
+    <t>10036-6524</t>
+  </si>
+  <si>
+    <t>1 S Jefferson St</t>
+  </si>
+  <si>
+    <t>Pulaski</t>
+  </si>
+  <si>
+    <t>13142-4703</t>
+  </si>
+  <si>
+    <t>164 Lake St</t>
+  </si>
+  <si>
+    <t>Rouses Point</t>
+  </si>
+  <si>
+    <t>12979-1427</t>
+  </si>
+  <si>
+    <t>4243 Hunt Rd</t>
+  </si>
+  <si>
+    <t>45242-6645</t>
+  </si>
+  <si>
+    <t>4243 Hunt Rd Fl 3</t>
+  </si>
+  <si>
+    <t>45242-6657</t>
+  </si>
+  <si>
+    <t>1313 N Bayshore Dr # 1</t>
+  </si>
+  <si>
+    <t>Coos Bay</t>
+  </si>
+  <si>
+    <t>97420-3197</t>
+  </si>
+  <si>
+    <t>315 W Main St</t>
+  </si>
+  <si>
+    <t>Enterprise</t>
+  </si>
+  <si>
+    <t>97828-1245</t>
+  </si>
+  <si>
+    <t>754 E 13th Ave</t>
+  </si>
+  <si>
+    <t>Eugene</t>
+  </si>
+  <si>
+    <t>97401-3743</t>
+  </si>
+  <si>
+    <t>7401 Airport Rd</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>18014-8810</t>
+  </si>
+  <si>
+    <t>15 Chestnut St</t>
+  </si>
+  <si>
+    <t>Carnegie</t>
+  </si>
+  <si>
+    <t>15106-2014</t>
+  </si>
+  <si>
+    <t>10200 Allentown Blvd</t>
+  </si>
+  <si>
+    <t>Grantville</t>
+  </si>
+  <si>
+    <t>17028-8718</t>
+  </si>
+  <si>
+    <t>6170 Morgantown Rd</t>
+  </si>
+  <si>
+    <t>Morgantown</t>
+  </si>
+  <si>
+    <t>19543-9564</t>
+  </si>
+  <si>
+    <t>200 S Broad St</t>
+  </si>
+  <si>
+    <t>19102-3803</t>
+  </si>
+  <si>
+    <t>441 N 5th St Fl 4</t>
+  </si>
+  <si>
+    <t>19123-4010</t>
+  </si>
+  <si>
+    <t>666 Centreville Pike</t>
+  </si>
+  <si>
+    <t>Slippery Rock</t>
+  </si>
+  <si>
+    <t>16057-3006</t>
+  </si>
+  <si>
+    <t>27 George St</t>
+  </si>
+  <si>
+    <t>Charleston</t>
+  </si>
+  <si>
+    <t>29401-1433</t>
+  </si>
+  <si>
+    <t>7525 Two Notch Rd</t>
+  </si>
+  <si>
+    <t>29223-6219</t>
+  </si>
+  <si>
+    <t>3629 E Parkway</t>
+  </si>
+  <si>
+    <t>Gatlinburg</t>
+  </si>
+  <si>
+    <t>37738-6208</t>
+  </si>
+  <si>
+    <t>455 Industrial Blvd Ste C</t>
+  </si>
+  <si>
+    <t>La Vergne</t>
+  </si>
+  <si>
+    <t>37086-4196</t>
+  </si>
+  <si>
+    <t>7909 Poplar Springs Rd</t>
+  </si>
+  <si>
+    <t>Loudon</t>
+  </si>
+  <si>
+    <t>37774-4427</t>
+  </si>
+  <si>
+    <t>6306 Millwood Ct</t>
+  </si>
+  <si>
+    <t>Arlington</t>
+  </si>
+  <si>
+    <t>76016-2665</t>
+  </si>
+  <si>
+    <t>200 Lavaca St</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>78701-3928</t>
+  </si>
+  <si>
+    <t>6593 Ih 37</t>
+  </si>
+  <si>
+    <t>Corpus Christi</t>
+  </si>
+  <si>
+    <t>78409-2715</t>
+  </si>
+  <si>
+    <t>201 S Washington St</t>
+  </si>
+  <si>
+    <t>Fredericksburg</t>
+  </si>
+  <si>
+    <t>78624-4632</t>
+  </si>
+  <si>
+    <t>19219 Katy Fwy Ste 200</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>77094-1053</t>
+  </si>
+  <si>
+    <t>1001 E Mccarty Ln</t>
+  </si>
+  <si>
+    <t>San Marcos</t>
+  </si>
+  <si>
+    <t>78666-1080</t>
+  </si>
+  <si>
+    <t>247 24th St</t>
+  </si>
+  <si>
+    <t>Ogden</t>
+  </si>
+  <si>
+    <t>84401-1425</t>
+  </si>
+  <si>
+    <t>14750 Conference Center Dr</t>
+  </si>
+  <si>
+    <t>20151-3800</t>
+  </si>
+  <si>
+    <t>223 Riverview Dr Ste A</t>
+  </si>
+  <si>
+    <t>Danville</t>
+  </si>
+  <si>
+    <t>24541-3435</t>
+  </si>
+  <si>
+    <t>2007 N Hamilton St</t>
+  </si>
+  <si>
+    <t>23230-4103</t>
+  </si>
+  <si>
+    <t>1307 Goshen Ripton Rd</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>05733-8463</t>
+  </si>
+  <si>
+    <t>1633 N Bayshore Dr # A</t>
+  </si>
+  <si>
+    <t>33132-1215</t>
+  </si>
+  <si>
+    <t>3355 Las Vegas Blvd S</t>
+  </si>
+  <si>
+    <t>89109-8941</t>
+  </si>
+  <si>
+    <t>748 Mcmechen St</t>
+  </si>
+  <si>
+    <t>Benwood</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>26031-1100</t>
+  </si>
+  <si>
+    <t>2050 University Ave</t>
+  </si>
+  <si>
+    <t>Palo Alto</t>
+  </si>
+  <si>
+    <t>94303-2248</t>
+  </si>
+  <si>
+    <t>6633 Main St</t>
+  </si>
+  <si>
+    <t>Mackinac Island</t>
+  </si>
+  <si>
+    <t>16300 Nyemii Pass Rd</t>
+  </si>
+  <si>
+    <t>Valley Center</t>
+  </si>
+  <si>
+    <t>92082-6769</t>
+  </si>
+  <si>
+    <t>Po Box 1005</t>
+  </si>
+  <si>
+    <t>63090-8005</t>
+  </si>
+  <si>
+    <t>2333 Seaway Blvd</t>
+  </si>
+  <si>
+    <t>Everett</t>
+  </si>
+  <si>
+    <t>98203-5902</t>
+  </si>
+  <si>
+    <t>2046 Parkway</t>
+  </si>
+  <si>
+    <t>Pigeon Forge</t>
+  </si>
+  <si>
+    <t>37863-2959</t>
+  </si>
+  <si>
+    <t>Po Box 769539</t>
+  </si>
+  <si>
+    <t>Roswell</t>
+  </si>
+  <si>
+    <t>30076-8222</t>
+  </si>
+  <si>
+    <t>6903 Rockledge Dr Ste 1500</t>
+  </si>
+  <si>
+    <t>20817-1862</t>
+  </si>
+  <si>
+    <t>687 Main St</t>
+  </si>
+  <si>
+    <t>Ogunquit</t>
+  </si>
+  <si>
+    <t>7036 Grand Geneva Way</t>
+  </si>
+  <si>
+    <t>Lake Geneva</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>53147-5105</t>
+  </si>
+  <si>
+    <t>14800 Landmark Blvd Ste 800</t>
+  </si>
+  <si>
+    <t>75254-7506</t>
+  </si>
+  <si>
+    <t>Third &amp; Spring Sts</t>
+  </si>
+  <si>
+    <t>3590 Grandview Pkwy</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>35243-1946</t>
+  </si>
+  <si>
+    <t>239 Central Ave</t>
+  </si>
+  <si>
+    <t>Hot Springs National Park</t>
+  </si>
+  <si>
+    <t>71901-3544</t>
+  </si>
+  <si>
+    <t>2398 E Camelback Rd Ste 1000</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>85016-9022</t>
+  </si>
+  <si>
+    <t>Po Box 700</t>
+  </si>
+  <si>
+    <t>Whiteriver</t>
+  </si>
+  <si>
+    <t>85941-0700</t>
+  </si>
+  <si>
+    <t>7667 Center Ave</t>
+  </si>
+  <si>
+    <t>Huntington Beach</t>
+  </si>
+  <si>
+    <t>92647-3073</t>
+  </si>
+  <si>
+    <t>6225 W Century Blvd</t>
+  </si>
+  <si>
+    <t>90045-5311</t>
+  </si>
+  <si>
+    <t>1775 Hancock St Ste 200</t>
+  </si>
+  <si>
+    <t>92110-2036</t>
+  </si>
+  <si>
+    <t>421 W B St</t>
+  </si>
+  <si>
+    <t>92101-3501</t>
+  </si>
+  <si>
+    <t>500 Hotel Cir N</t>
+  </si>
+  <si>
+    <t>92108-3005</t>
+  </si>
+  <si>
+    <t>433 California St Ste 700</t>
+  </si>
+  <si>
+    <t>94104-2011</t>
+  </si>
+  <si>
+    <t>1350 17th St Ste 150</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>80202-1525</t>
+  </si>
+  <si>
+    <t>321 17th St</t>
+  </si>
+  <si>
+    <t>80202-4099</t>
+  </si>
+  <si>
+    <t>1672 Fish Hatchery Rd</t>
+  </si>
+  <si>
+    <t>Estes Park</t>
+  </si>
+  <si>
+    <t>3801 Automation Way Ste 100</t>
+  </si>
+  <si>
+    <t>Fort Collins</t>
+  </si>
+  <si>
+    <t>80525-5735</t>
+  </si>
+  <si>
+    <t>Po Box 4016</t>
+  </si>
+  <si>
+    <t>Granby</t>
+  </si>
+  <si>
+    <t>80446-4016</t>
+  </si>
+  <si>
+    <t>1847 Ski Time Square Dr</t>
+  </si>
+  <si>
+    <t>Steamboat Springs</t>
+  </si>
+  <si>
+    <t>229 George St</t>
+  </si>
+  <si>
+    <t>New Haven</t>
+  </si>
+  <si>
+    <t>06510-3200</t>
+  </si>
+  <si>
+    <t>1515 S Atlantic Ave</t>
+  </si>
+  <si>
+    <t>32118-4954</t>
+  </si>
+  <si>
+    <t>699 5th Ave S</t>
+  </si>
+  <si>
+    <t>Naples</t>
+  </si>
+  <si>
+    <t>34102-6601</t>
+  </si>
+  <si>
+    <t>3720 Sw College Rd</t>
+  </si>
+  <si>
+    <t>Ocala</t>
+  </si>
+  <si>
+    <t>34474-4441</t>
+  </si>
+  <si>
+    <t>4120 Central Florida Pkwy</t>
+  </si>
+  <si>
+    <t>1200 S Ocean Blvd</t>
+  </si>
+  <si>
+    <t>Pompano Beach</t>
+  </si>
+  <si>
+    <t>33062-6698</t>
+  </si>
+  <si>
+    <t>1200 W Retta Esplanade Ste 57a</t>
+  </si>
+  <si>
+    <t>Punta Gorda</t>
+  </si>
+  <si>
+    <t>33950-5377</t>
+  </si>
+  <si>
+    <t>1111 Ritz Carlton Dr</t>
+  </si>
+  <si>
+    <t>Sarasota</t>
+  </si>
+  <si>
+    <t>34236-5594</t>
+  </si>
+  <si>
+    <t>7125 Fruitville Rd # 1171</t>
+  </si>
+  <si>
+    <t>34240-8995</t>
+  </si>
+  <si>
+    <t>7627 W Courtney Campbell Cswy</t>
+  </si>
+  <si>
+    <t>Tampa</t>
+  </si>
+  <si>
+    <t>33607-1431</t>
+  </si>
+  <si>
+    <t>13305 Tampa Oaks Blvd</t>
+  </si>
+  <si>
+    <t>Temple Terrace</t>
+  </si>
+  <si>
+    <t>33637-1110</t>
+  </si>
+  <si>
+    <t>145 Cliftwood Dr</t>
+  </si>
+  <si>
+    <t>30328-4840</t>
+  </si>
+  <si>
+    <t>7336 Bear Ln</t>
+  </si>
+  <si>
+    <t>31909-2516</t>
   </si>
 </sst>
 </file>
@@ -1911,10 +2838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D374"/>
+  <dimension ref="A1:D554"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+      <selection activeCell="D159" sqref="A1:D554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -7158,6 +8085,2526 @@
       </c>
       <c r="D374" s="2" t="s">
         <v>522</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4">
+      <c r="A375" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4">
+      <c r="A376" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B376" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4">
+      <c r="A377" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B377" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4">
+      <c r="A378" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4">
+      <c r="A379" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B379" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4">
+      <c r="A380" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B380" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="C380" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D380" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4">
+      <c r="A381" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C381" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D381" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4">
+      <c r="A382" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D382" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4">
+      <c r="A383" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4">
+      <c r="A384" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B384" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D384" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4">
+      <c r="A385" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C385" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D385" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4">
+      <c r="A386" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B386" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C386" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D386" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4">
+      <c r="A387" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B387" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C387" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D387" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4">
+      <c r="A388" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C388" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D388" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4">
+      <c r="A389" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B389" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D389" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4">
+      <c r="A390" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B390" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D390" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4">
+      <c r="A391" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B391" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D391" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4">
+      <c r="A392" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D392" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4">
+      <c r="A393" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D393" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4">
+      <c r="A394" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B394" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C394" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D394" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4">
+      <c r="A395" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4">
+      <c r="A396" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4">
+      <c r="A397" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4">
+      <c r="A398" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B398" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C398" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D398" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4">
+      <c r="A399" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B399" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C399" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D399" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4">
+      <c r="A400" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B400" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C400" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D400" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4">
+      <c r="A401" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B401" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C401" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D401" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4">
+      <c r="A402" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B402" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D402" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4">
+      <c r="A403" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4">
+      <c r="A404" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B404" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4">
+      <c r="A405" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="B405" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C405" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D405" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4">
+      <c r="A406" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="B406" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C406" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D406" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4">
+      <c r="A407" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="B407" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D407" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4">
+      <c r="A408" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B408" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C408" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D408" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4">
+      <c r="A409" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B409" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4">
+      <c r="A410" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B410" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C410" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D410" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4">
+      <c r="A411" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B411" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C411" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4">
+      <c r="A412" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B412" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C412" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D412" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4">
+      <c r="A413" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B413" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C413" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D413" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4">
+      <c r="A414" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B414" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C414" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D414" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4">
+      <c r="A415" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B415" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C415" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D415" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4">
+      <c r="A416" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B416" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="C416" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D416" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4">
+      <c r="A417" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="B417" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="C417" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D417" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4">
+      <c r="A418" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B418" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C418" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D418" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4">
+      <c r="A419" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B419" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C419" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D419" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4">
+      <c r="A420" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B420" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C420" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D420" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4">
+      <c r="A421" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B421" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C421" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D421" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4">
+      <c r="A422" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="B422" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C422" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D422" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4">
+      <c r="A423" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B423" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C423" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D423" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4">
+      <c r="A424" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="B424" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C424" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D424" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4">
+      <c r="A425" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B425" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C425" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D425" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4">
+      <c r="A426" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="B426" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C426" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D426" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4">
+      <c r="A427" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B427" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C427" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D427" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4">
+      <c r="A428" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="B428" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="C428" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D428" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4">
+      <c r="A429" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B429" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C429" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D429" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4">
+      <c r="A430" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B430" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C430" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D430" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4">
+      <c r="A431" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="B431" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C431" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D431" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4">
+      <c r="A432" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B432" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C432" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D432" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4">
+      <c r="A433" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="B433" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="C433" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D433" s="2" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4">
+      <c r="A434" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="B434" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="C434" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D434" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4">
+      <c r="A435" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="B435" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C435" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="D435" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4">
+      <c r="A436" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B436" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="C436" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D436" s="2">
+        <v>89311</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4">
+      <c r="A437" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="B437" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="C437" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D437" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4">
+      <c r="A438" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="B438" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="C438" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D438" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4">
+      <c r="A439" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="B439" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="C439" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D439" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4">
+      <c r="A440" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="B440" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="C440" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D440" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4">
+      <c r="A441" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="B441" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="C441" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D441" s="2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4">
+      <c r="A442" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="B442" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C442" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D442" s="2" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4">
+      <c r="A443" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="B443" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C443" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D443" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4">
+      <c r="A444" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="B444" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C444" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D444" s="2">
+        <v>10013</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4">
+      <c r="A445" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="B445" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C445" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D445" s="2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4">
+      <c r="A446" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="B446" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="C446" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D446" s="2" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4">
+      <c r="A447" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B447" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="C447" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D447" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4">
+      <c r="A448" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="B448" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C448" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D448" s="2" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4">
+      <c r="A449" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="B449" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C449" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D449" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4">
+      <c r="A450" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="B450" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C450" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D450" s="2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4">
+      <c r="A451" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="B451" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="C451" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D451" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4">
+      <c r="A452" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="B452" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="C452" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D452" s="2" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4">
+      <c r="A453" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="B453" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="C453" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D453" s="2" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4">
+      <c r="A454" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="B454" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="C454" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D454" s="2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4">
+      <c r="A455" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="B455" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="C455" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D455" s="2" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4">
+      <c r="A456" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="B456" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="C456" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D456" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4">
+      <c r="A457" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="B457" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C457" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D457" s="2" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4">
+      <c r="A458" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B458" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C458" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D458" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4">
+      <c r="A459" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="B459" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="C459" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D459" s="2" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4">
+      <c r="A460" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="B460" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="C460" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D460" s="2" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4">
+      <c r="A461" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B461" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C461" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D461" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4">
+      <c r="A462" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B462" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C462" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D462" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4">
+      <c r="A463" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B463" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C463" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D463" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4">
+      <c r="A464" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B464" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C464" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D464" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4">
+      <c r="A465" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B465" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C465" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D465" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4">
+      <c r="A466" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="B466" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C466" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D466" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4">
+      <c r="A467" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="B467" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C467" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D467" s="2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4">
+      <c r="A468" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B468" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C468" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D468" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4">
+      <c r="A469" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B469" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C469" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D469" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4">
+      <c r="A470" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B470" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C470" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D470" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4">
+      <c r="A471" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B471" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C471" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D471" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4">
+      <c r="A472" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B472" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C472" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D472" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4">
+      <c r="A473" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="B473" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="C473" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D473" s="2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4">
+      <c r="A474" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="B474" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="C474" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D474" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4">
+      <c r="A475" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="B475" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="C475" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D475" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4">
+      <c r="A476" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="B476" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="C476" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D476" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4">
+      <c r="A477" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="B477" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="C477" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D477" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4">
+      <c r="A478" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B478" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="C478" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D478" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4">
+      <c r="A479" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="B479" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="C479" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D479" s="2" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4">
+      <c r="A480" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="B480" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C480" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D480" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4">
+      <c r="A481" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B481" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C481" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D481" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4">
+      <c r="A482" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="B482" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="C482" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D482" s="2" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4">
+      <c r="A483" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B483" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C483" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D483" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4">
+      <c r="A484" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B484" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C484" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D484" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4">
+      <c r="A485" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="B485" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="C485" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D485" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4">
+      <c r="A486" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B486" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C486" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D486" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4">
+      <c r="A487" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B487" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C487" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D487" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4">
+      <c r="A488" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B488" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C488" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D488" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4">
+      <c r="A489" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B489" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="C489" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D489" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4">
+      <c r="A490" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="B490" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C490" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D490" s="2" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4">
+      <c r="A491" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B491" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C491" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D491" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4">
+      <c r="A492" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B492" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C492" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D492" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4">
+      <c r="A493" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B493" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C493" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D493" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4">
+      <c r="A494" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B494" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C494" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D494" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4">
+      <c r="A495" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B495" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C495" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D495" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4">
+      <c r="A496" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B496" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C496" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D496" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4">
+      <c r="A497" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B497" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C497" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D497" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4">
+      <c r="A498" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="B498" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C498" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D498" s="2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4">
+      <c r="A499" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="B499" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="C499" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="D499" s="2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4">
+      <c r="A500" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="B500" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="C500" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D500" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4">
+      <c r="A501" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="B501" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="C501" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D501" s="2">
+        <v>49757</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4">
+      <c r="A502" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="B502" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C502" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D502" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4">
+      <c r="A503" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B503" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C503" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D503" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4">
+      <c r="A504" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B504" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C504" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D504" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4">
+      <c r="A505" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="B505" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C505" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D505" s="2" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4">
+      <c r="A506" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C506" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D506" s="2" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4">
+      <c r="A507" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B507" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C507" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D507" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4">
+      <c r="A508" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="B508" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C508" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D508" s="2" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4">
+      <c r="A509" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="B509" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="C509" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D509" s="2" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4">
+      <c r="A510" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B510" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C510" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D510" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4">
+      <c r="A511" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="B511" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="C511" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D511" s="2" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4">
+      <c r="A512" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B512" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C512" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D512" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4">
+      <c r="A513" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B513" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C513" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D513" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4">
+      <c r="A514" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="B514" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C514" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D514" s="2" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4">
+      <c r="A515" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B515" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="C515" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D515" s="2">
+        <v>3907</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4">
+      <c r="A516" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B516" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C516" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D516" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4">
+      <c r="A517" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B517" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C517" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D517" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4">
+      <c r="A518" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="B518" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="C518" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="D518" s="2" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4">
+      <c r="A519" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B519" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C519" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D519" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4">
+      <c r="A520" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="B520" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C520" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D520" s="2" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4">
+      <c r="A521" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="B521" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C521" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D521" s="2">
+        <v>99840</v>
+      </c>
+    </row>
+    <row r="522" spans="1:4">
+      <c r="A522" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="B522" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="C522" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D522" s="2" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4">
+      <c r="A523" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="B523" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="C523" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D523" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="524" spans="1:4">
+      <c r="A524" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="B524" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="C524" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D524" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="525" spans="1:4">
+      <c r="A525" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="B525" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="C525" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D525" s="2" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="526" spans="1:4">
+      <c r="A526" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="B526" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="C526" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D526" s="2" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="527" spans="1:4">
+      <c r="A527" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B527" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C527" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D527" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="528" spans="1:4">
+      <c r="A528" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="B528" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="C528" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D528" s="2" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="529" spans="1:4">
+      <c r="A529" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="B529" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C529" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D529" s="2" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4">
+      <c r="A530" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="B530" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C530" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D530" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="531" spans="1:4">
+      <c r="A531" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="B531" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C531" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D531" s="2" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4">
+      <c r="A532" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="B532" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C532" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D532" s="2" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4">
+      <c r="A533" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="B533" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C533" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D533" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4">
+      <c r="A534" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="B534" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="C534" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D534" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4">
+      <c r="A535" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="B535" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="C535" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D535" s="2" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4">
+      <c r="A536" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="B536" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C536" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D536" s="2">
+        <v>80517</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4">
+      <c r="A537" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="B537" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="C537" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D537" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4">
+      <c r="A538" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="B538" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="C538" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D538" s="2" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4">
+      <c r="A539" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="B539" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="C539" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D539" s="2">
+        <v>80487</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4">
+      <c r="A540" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="B540" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="C540" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D540" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4">
+      <c r="A541" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="B541" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C541" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D541" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4">
+      <c r="A542" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B542" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C542" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D542" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4">
+      <c r="A543" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B543" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="C543" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D543" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4">
+      <c r="A544" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="B544" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="C544" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D544" s="2" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4">
+      <c r="A545" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B545" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C545" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D545" s="2">
+        <v>32819</v>
+      </c>
+    </row>
+    <row r="546" spans="1:4">
+      <c r="A546" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="B546" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="C546" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D546" s="2" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4">
+      <c r="A547" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="B547" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="C547" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D547" s="2" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4">
+      <c r="A548" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="B548" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="C548" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D548" s="2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4">
+      <c r="A549" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B549" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="C549" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D549" s="2" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4">
+      <c r="A550" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B550" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="C550" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D550" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4">
+      <c r="A551" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="B551" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="C551" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D551" s="2" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4">
+      <c r="A552" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B552" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C552" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D552" s="2" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4">
+      <c r="A553" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B553" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C553" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D553" s="2" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4">
+      <c r="A554" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B554" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C554" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D554" s="2" t="s">
+        <v>831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>